<commit_message>
✨ feat: update form and UI
</commit_message>
<xml_diff>
--- a/app/static/docs/sample.xlsx
+++ b/app/static/docs/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\prediksi-kelulusan-mahasiswa\app\static\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228DBD81-BD66-4CCA-8D46-83495F9A0DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA50C8C-19AE-4744-AE06-159A58AB8721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB26FC7F-1FDF-4AD8-A82C-1B937DF9A7F5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{FB26FC7F-1FDF-4AD8-A82C-1B937DF9A7F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,26 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>asal_sma</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>penghasilan_orang_tua</t>
   </si>
   <si>
-    <t>toefl</t>
-  </si>
-  <si>
     <t>prodi</t>
   </si>
   <si>
-    <t>jalur_masuk</t>
-  </si>
-  <si>
-    <t>jenis_kelamin</t>
-  </si>
-  <si>
     <t>ip_semester_1</t>
   </si>
   <si>
@@ -68,47 +56,23 @@
     <t>ip_semester_4</t>
   </si>
   <si>
-    <t>ip_semester_5</t>
-  </si>
-  <si>
-    <t>ip_semester_6</t>
-  </si>
-  <si>
-    <t>ip_semester_7</t>
-  </si>
-  <si>
-    <t>ip_semester_8</t>
-  </si>
-  <si>
-    <t>ip_semester_9</t>
-  </si>
-  <si>
-    <t>ip_semester_10</t>
-  </si>
-  <si>
-    <t>ip_semester_11</t>
-  </si>
-  <si>
-    <t>ip_semester_12</t>
-  </si>
-  <si>
-    <t>ip_semester_13</t>
-  </si>
-  <si>
-    <t>ip_semester_14</t>
-  </si>
-  <si>
     <t>nim</t>
   </si>
   <si>
     <t>nama</t>
+  </si>
+  <si>
+    <t>nama_sma</t>
+  </si>
+  <si>
+    <t>jalur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +85,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF98C379"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,8 +113,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,96 +452,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A1C1F6-92A5-4752-881F-F96F371D1E43}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
🛠️ fix: ipk condition
</commit_message>
<xml_diff>
--- a/app/static/docs/sample.xlsx
+++ b/app/static/docs/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\prediksi-kelulusan-mahasiswa\app\static\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA50C8C-19AE-4744-AE06-159A58AB8721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42DB98A-32A4-48B5-BB67-D11C503C3409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{FB26FC7F-1FDF-4AD8-A82C-1B937DF9A7F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB26FC7F-1FDF-4AD8-A82C-1B937DF9A7F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>penghasilan_orang_tua</t>
   </si>
@@ -66,13 +66,79 @@
   </si>
   <si>
     <t>jalur</t>
+  </si>
+  <si>
+    <t>SMK Negeri 1 Siatasbarita</t>
+  </si>
+  <si>
+    <t>Teknologi Komputer</t>
+  </si>
+  <si>
+    <t>UTBK</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Hesoyam</t>
+  </si>
+  <si>
+    <t>Aezakmi</t>
+  </si>
+  <si>
+    <t>SMA Negri 1 Sidamanik</t>
+  </si>
+  <si>
+    <t>Manajemen Rekayasa</t>
+  </si>
+  <si>
+    <t>PMDK</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>Uzumymw</t>
+  </si>
+  <si>
+    <t>SMAN 4 BINJAI</t>
+  </si>
+  <si>
+    <t>Teknik Bioproses</t>
+  </si>
+  <si>
+    <t>USM3</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>2.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,12 +151,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF98C379"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,11 +173,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,21 +509,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A1C1F6-92A5-4752-881F-F96F371D1E43}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -502,14 +560,100 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="A2">
+        <v>12345</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>5000000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="A3">
+        <v>23456</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>12000000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>34567</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>2000000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>